<commit_message>
23.05.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/May/All Details/22.05.2020/MC Balance Transfer May 2020.xlsx
+++ b/2020/May/All Details/22.05.2020/MC Balance Transfer May 2020.xlsx
@@ -1485,9 +1485,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>